<commit_message>
Correct rem file location
</commit_message>
<xml_diff>
--- a/organize free cities files live.xlsx
+++ b/organize free cities files live.xlsx
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F363"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="F243" sqref="F243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5588,7 +5588,7 @@
         <v>364</v>
       </c>
       <c r="F242" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>